<commit_message>
Hotfixes and refactoring before defence.
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Svetoslav\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\SPASocialNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -368,10 +368,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,11 +722,11 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -801,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D14" s="5">
         <v>10</v>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>